<commit_message>
Menambahkan file model_1.1.h5 dan memperbarui sprint_project
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sin\KOLEAH\SMT 7\ML\Tubes\TubesPrakML-243-264\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\A-Semester 7\Pembelajaran Mesin D - Pak Yufis\TubesPrak-243-264\TubesPrakML-243-264\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09E38B18-FA18-4E78-8CFD-DFEBB75F67F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B5BD87-2233-4D3C-B4BF-E96119547202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11520" xr2:uid="{9DCC8ECD-33F0-48B2-845D-B02D9229471A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9DCC8ECD-33F0-48B2-845D-B02D9229471A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -70,13 +70,28 @@
   </si>
   <si>
     <t>Membangun Model 2</t>
+  </si>
+  <si>
+    <t>Splitting Dataset + Augmentasi untuk Oversampling Model 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 Nov 21 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 Nov 21 </t>
+  </si>
+  <si>
+    <t>Splitting Dataset + Augmentasi untuk Oversampling Model 2</t>
+  </si>
+  <si>
+    <t>Waiting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -91,6 +106,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -141,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -157,6 +179,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BB09BE-0A17-4E47-A9B9-53F8A1097084}">
-  <dimension ref="B2:G8"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G8"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -483,7 +517,7 @@
     <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -626,7 +660,48 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="8">
+        <v>44506</v>
+      </c>
+      <c r="D9" s="8">
+        <v>44510</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8">
+        <v>44507</v>
+      </c>
+      <c r="D10" s="8">
+        <v>44510</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Merapikan ulang dokumentasi progres
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KULIAH\A-Semester 7\Pembelajaran Mesin D - Pak Yufis\TubesPrak-243-264\TubesPrakML-243-264\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sin\KOLEAH\SMT 7\ML\Tubes\TubesPrakML-243-264\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B5BD87-2233-4D3C-B4BF-E96119547202}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD847EB-5288-485E-BC96-B49D8A44EF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{9DCC8ECD-33F0-48B2-845D-B02D9229471A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11520" xr2:uid="{9DCC8ECD-33F0-48B2-845D-B02D9229471A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -84,7 +84,7 @@
     <t>Splitting Dataset + Augmentasi untuk Oversampling Model 2</t>
   </si>
   <si>
-    <t>Waiting</t>
+    <t>No.</t>
   </si>
 </sst>
 </file>
@@ -163,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -191,6 +191,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,47 +506,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BB09BE-0A17-4E47-A9B9-53F8A1097084}">
-  <dimension ref="B2:G10"/>
+  <dimension ref="B2:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="6">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" s="3">
-        <v>44479</v>
       </c>
       <c r="D3" s="3">
         <v>44479</v>
@@ -553,19 +557,22 @@
       <c r="E3" s="3">
         <v>44479</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3">
+        <v>44479</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="3">
-        <v>44480</v>
       </c>
       <c r="D4" s="3">
         <v>44480</v>
@@ -573,131 +580,152 @@
       <c r="E4" s="3">
         <v>44480</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3">
+        <v>44480</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="1" t="s">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="6">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="3">
         <v>44483</v>
-      </c>
-      <c r="D5" s="3">
-        <v>44494</v>
       </c>
       <c r="E5" s="3">
         <v>44494</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3">
+        <v>44494</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="6">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="5">
         <v>44485</v>
-      </c>
-      <c r="D6" s="5">
-        <v>44495</v>
       </c>
       <c r="E6" s="5">
         <v>44495</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="5">
+        <v>44495</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="6">
+        <v>5</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>44493</v>
-      </c>
-      <c r="D7" s="5">
-        <v>44495</v>
       </c>
       <c r="E7" s="5">
         <v>44495</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="5">
+        <v>44495</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>6</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>44493</v>
-      </c>
-      <c r="D8" s="5">
-        <v>44495</v>
       </c>
       <c r="E8" s="5">
         <v>44495</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="5">
+        <v>44495</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="H8" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
+    <row r="9" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B9" s="6">
+        <v>7</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="8">
+      <c r="D9" s="8">
         <v>44506</v>
       </c>
-      <c r="D9" s="8">
+      <c r="E9" s="8">
         <v>44510</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="H9" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
+    <row r="10" spans="2:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <v>8</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="8">
+      <c r="D10" s="8">
         <v>44507</v>
       </c>
-      <c r="D10" s="8">
+      <c r="E10" s="8">
         <v>44510</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="F10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="G10" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="4" t="s">
-        <v>19</v>
+      <c r="H10" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Membuat ulang dan evaluasi model 2
</commit_message>
<xml_diff>
--- a/sprint_project.xlsx
+++ b/sprint_project.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sin\KOLEAH\SMT 7\ML\Tubes\TubesPrakML-243-264\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD847EB-5288-485E-BC96-B49D8A44EF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{495F8C6A-9E68-4C89-84EE-7E60461AB31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11520" xr2:uid="{9DCC8ECD-33F0-48B2-845D-B02D9229471A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -85,6 +85,18 @@
   </si>
   <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Membangun ulang Model 1 </t>
+  </si>
+  <si>
+    <t>Membangun ulang Model 2</t>
+  </si>
+  <si>
+    <t>Evaluasi Model 1</t>
+  </si>
+  <si>
+    <t>Evaluasi Model 2</t>
   </si>
 </sst>
 </file>
@@ -136,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -159,11 +171,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -192,6 +230,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17BB09BE-0A17-4E47-A9B9-53F8A1097084}">
-  <dimension ref="B2:H10"/>
+  <dimension ref="B2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,8 +726,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
+    <row r="9" spans="2:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="12">
         <v>7</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -705,10 +749,8 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="2:8" ht="90" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <v>8</v>
-      </c>
+    <row r="10" spans="2:8" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="13"/>
       <c r="C10" s="7" t="s">
         <v>18</v>
       </c>
@@ -728,7 +770,100 @@
         <v>12</v>
       </c>
     </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="12">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="8">
+        <v>44513</v>
+      </c>
+      <c r="E11" s="8">
+        <v>44517</v>
+      </c>
+      <c r="F11" s="8">
+        <v>44518</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="13"/>
+      <c r="C12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8">
+        <v>44513</v>
+      </c>
+      <c r="E12" s="8">
+        <v>44517</v>
+      </c>
+      <c r="F12" s="8">
+        <v>44518</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="12">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="8">
+        <v>44519</v>
+      </c>
+      <c r="E13" s="8">
+        <v>44520</v>
+      </c>
+      <c r="F13" s="8">
+        <v>44521</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="13"/>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="8">
+        <v>44519</v>
+      </c>
+      <c r="E14" s="8">
+        <v>44520</v>
+      </c>
+      <c r="F14" s="8">
+        <v>44521</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>